<commit_message>
Fixed Bug in Data Access Layer
</commit_message>
<xml_diff>
--- a/Progress/DataAccessLayer.xlsx
+++ b/Progress/DataAccessLayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Driving-License-Management-Desktop-App\Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EED66F-1ADB-4CE3-8B92-5DFE23D32D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E0DEC9-B083-4992-83E2-56C0C5E6F992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="118">
   <si>
     <t>Class Name</t>
   </si>
@@ -396,9 +396,6 @@
   </si>
   <si>
     <t>Implementation</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -575,13 +572,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -597,6 +587,13 @@
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -878,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="97" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="97" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,11 +957,11 @@
       </c>
       <c r="I4" s="9">
         <f>(COUNTIF(D2:D999,"Done"))/(COUNTIF(D2:D999,"Done") + COUNTIF(D2:D999,"Not Started") + COUNTIF(D2:D999,"Implemented"))</f>
-        <v>0.14893617021276595</v>
+        <v>0.18947368421052632</v>
       </c>
       <c r="J4" s="9">
         <f>(COUNTIF(E2:E999,"Done"))/(COUNTIF(E2:E999,"Done") + COUNTIF(E2:E999,"Not Started") + COUNTIF(D2:D999,"Implemented") + COUNTIF(E2:E999,"Failed"))</f>
-        <v>0.14736842105263157</v>
+        <v>0.18947368421052632</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1130,10 +1127,10 @@
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1169,10 +1166,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1182,10 +1179,10 @@
         <v>20</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1195,10 +1192,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2347,6 +2344,24 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="B53:B62"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="B64:B71"/>
+    <mergeCell ref="A63:A71"/>
     <mergeCell ref="B93:B104"/>
     <mergeCell ref="A92:A104"/>
     <mergeCell ref="B106:B110"/>
@@ -2357,47 +2372,29 @@
     <mergeCell ref="A79:A86"/>
     <mergeCell ref="B88:B91"/>
     <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="B53:B62"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="B64:B71"/>
-    <mergeCell ref="A63:A71"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B9:B18"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B20:B22"/>
   </mergeCells>
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2:E18 D20:E30 D32:E43 D45:E62 D64:E78 D80:E91 D93:E104 D106:E1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E18 E20:E30 E32:E43 E45:E62 E64:E78 E80:E91 E93:E104 E106:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E18 E20:E30 E32:E43 E45:E62 E64:E78 E80:E91 E93:E104 E106:E1048576" xr:uid="{855525DE-213F-45D8-9587-64AA93ECBAA2}">
       <formula1>"Done,Failed,Not Started,Implemented"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Implemented All planned Methods in Data Access Layer
</commit_message>
<xml_diff>
--- a/Progress/DataAccessLayer.xlsx
+++ b/Progress/DataAccessLayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Driving-License-Management-Desktop-App\Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E0DEC9-B083-4992-83E2-56C0C5E6F992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7816CB-0362-45FF-8B33-68602CCA61D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -353,9 +353,6 @@
     <t>public static bool IsUserExistForPersonID(int PersonID)</t>
   </si>
   <si>
-    <t>public static bool DoesPersonHaveUser44(int PersonID)</t>
-  </si>
-  <si>
     <t>public static bool ChangePassword(int UserID, string NewPassword)</t>
   </si>
   <si>
@@ -396,6 +393,9 @@
   </si>
   <si>
     <t>Implementation</t>
+  </si>
+  <si>
+    <t>public static bool DoesPersonHaveUser(int PersonID)</t>
   </si>
 </sst>
 </file>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="97" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="97" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,13 +902,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -931,16 +931,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -950,14 +950,14 @@
         <v>6</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I4" s="9">
         <f>(COUNTIF(D2:D999,"Done"))/(COUNTIF(D2:D999,"Done") + COUNTIF(D2:D999,"Not Started") + COUNTIF(D2:D999,"Implemented"))</f>
-        <v>0.18947368421052632</v>
+        <v>1</v>
       </c>
       <c r="J4" s="9">
         <f>(COUNTIF(E2:E999,"Done"))/(COUNTIF(E2:E999,"Done") + COUNTIF(E2:E999,"Not Started") + COUNTIF(D2:D999,"Implemented") + COUNTIF(E2:E999,"Failed"))</f>
@@ -971,10 +971,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -984,23 +984,23 @@
         <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="10"/>
       <c r="C7" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1020,13 +1020,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1036,10 +1036,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1049,10 +1049,10 @@
         <v>11</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1062,10 +1062,10 @@
         <v>23</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1075,10 +1075,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1088,10 +1088,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1101,10 +1101,10 @@
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1114,10 +1114,10 @@
         <v>15</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1127,10 +1127,10 @@
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1140,10 +1140,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1166,10 +1166,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1179,10 +1179,10 @@
         <v>20</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1192,10 +1192,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1218,10 +1218,10 @@
         <v>24</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1231,10 +1231,10 @@
         <v>25</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1244,10 +1244,10 @@
         <v>26</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1257,10 +1257,10 @@
         <v>27</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1270,10 +1270,10 @@
         <v>28</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1283,10 +1283,10 @@
         <v>29</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1296,10 +1296,10 @@
         <v>30</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1322,10 +1322,10 @@
         <v>32</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1335,10 +1335,10 @@
         <v>33</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1348,10 +1348,10 @@
         <v>34</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1361,10 +1361,10 @@
         <v>35</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1374,10 +1374,10 @@
         <v>36</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1400,10 +1400,10 @@
         <v>38</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1413,10 +1413,10 @@
         <v>39</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1426,10 +1426,10 @@
         <v>40</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1439,10 +1439,10 @@
         <v>41</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1452,10 +1452,10 @@
         <v>42</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1465,10 +1465,10 @@
         <v>43</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1491,10 +1491,10 @@
         <v>45</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1504,10 +1504,10 @@
         <v>46</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1517,10 +1517,10 @@
         <v>47</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1530,10 +1530,10 @@
         <v>48</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1543,10 +1543,10 @@
         <v>49</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1556,10 +1556,10 @@
         <v>50</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1569,10 +1569,10 @@
         <v>51</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1595,10 +1595,10 @@
         <v>53</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1608,10 +1608,10 @@
         <v>54</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1621,10 +1621,10 @@
         <v>55</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1634,10 +1634,10 @@
         <v>56</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1647,10 +1647,10 @@
         <v>57</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1660,10 +1660,10 @@
         <v>58</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1673,10 +1673,10 @@
         <v>59</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1686,10 +1686,10 @@
         <v>60</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1699,10 +1699,10 @@
         <v>61</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1712,10 +1712,10 @@
         <v>62</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1738,10 +1738,10 @@
         <v>64</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1751,10 +1751,10 @@
         <v>65</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1764,10 +1764,10 @@
         <v>66</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -1777,10 +1777,10 @@
         <v>67</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1790,10 +1790,10 @@
         <v>68</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1803,10 +1803,10 @@
         <v>69</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1816,10 +1816,10 @@
         <v>70</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1829,10 +1829,10 @@
         <v>71</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1855,10 +1855,10 @@
         <v>73</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1868,10 +1868,10 @@
         <v>74</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1881,10 +1881,10 @@
         <v>75</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1894,10 +1894,10 @@
         <v>76</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1907,10 +1907,10 @@
         <v>77</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1920,10 +1920,10 @@
         <v>78</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1946,10 +1946,10 @@
         <v>80</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1959,10 +1959,10 @@
         <v>81</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1972,10 +1972,10 @@
         <v>82</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1985,10 +1985,10 @@
         <v>83</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1998,10 +1998,10 @@
         <v>84</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2011,10 +2011,10 @@
         <v>85</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2024,10 +2024,10 @@
         <v>86</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2050,10 +2050,10 @@
         <v>88</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2063,10 +2063,10 @@
         <v>89</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2076,10 +2076,10 @@
         <v>90</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2089,10 +2089,10 @@
         <v>91</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2115,10 +2115,10 @@
         <v>93</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2128,10 +2128,10 @@
         <v>94</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2141,10 +2141,10 @@
         <v>95</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2154,10 +2154,10 @@
         <v>96</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2167,10 +2167,10 @@
         <v>97</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2180,10 +2180,10 @@
         <v>98</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2193,10 +2193,10 @@
         <v>99</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2206,10 +2206,10 @@
         <v>100</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -2219,10 +2219,10 @@
         <v>101</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -2232,41 +2232,41 @@
         <v>102</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
       <c r="B103" s="10"/>
       <c r="C103" s="7" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="13"/>
       <c r="B104" s="10"/>
       <c r="C104" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>2</v>
@@ -2281,65 +2281,65 @@
         <v>3</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="16"/>
       <c r="B107" s="14"/>
       <c r="C107" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="16"/>
       <c r="B108" s="14"/>
       <c r="C108" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
       <c r="B109" s="14"/>
       <c r="C109" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" s="17"/>
       <c r="B110" s="14"/>
       <c r="C110" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more Testing Methods and Classes
</commit_message>
<xml_diff>
--- a/Progress/DataAccessLayer.xlsx
+++ b/Progress/DataAccessLayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Driving-License-Management-Desktop-App\Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F894C0E1-28FB-4873-853C-DE583EFBE73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D539E3-10BB-444D-B4A6-4F1810C9A4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,8 +963,8 @@
         <v>1</v>
       </c>
       <c r="J4" s="9">
-        <f>(COUNTIF(E2:E999,"Done"))/(COUNTIF(E2:E999,"Done") + COUNTIF(E2:E999,"Not Started") + COUNTIF(D2:D999,"Implemented") + COUNTIF(E2:E999,"Failed"))</f>
-        <v>0.38297872340425532</v>
+        <f>(COUNTIF(E2:E999,"Done"))/(COUNTIF(E2:E999,"Done") + COUNTIF(E2:E999,"Not Started") + COUNTIF(E2:E999,"Implemented") + COUNTIF(E2:E999,"Failed"))</f>
+        <v>0.37894736842105264</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1510,7 +1510,7 @@
         <v>111</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1523,7 +1523,7 @@
         <v>111</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1536,7 +1536,7 @@
         <v>111</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1549,7 +1549,7 @@
         <v>111</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1562,7 +1562,7 @@
         <v>111</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1575,7 +1575,7 @@
         <v>111</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1601,7 +1601,7 @@
         <v>111</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1614,7 +1614,7 @@
         <v>111</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,7 +1627,7 @@
         <v>111</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1640,7 +1640,7 @@
         <v>111</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1653,7 +1653,7 @@
         <v>111</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1666,7 +1666,7 @@
         <v>111</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>111</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1692,7 +1692,7 @@
         <v>111</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1705,7 +1705,7 @@
         <v>111</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1718,7 +1718,7 @@
         <v>111</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1744,7 +1744,7 @@
         <v>111</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1757,7 +1757,7 @@
         <v>111</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1770,7 +1770,7 @@
         <v>111</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>111</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1796,7 +1796,7 @@
         <v>111</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1809,7 +1809,7 @@
         <v>111</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1822,7 +1822,7 @@
         <v>111</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1835,7 +1835,7 @@
         <v>111</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1861,7 +1861,7 @@
         <v>111</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1874,7 +1874,7 @@
         <v>111</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1887,7 +1887,7 @@
         <v>111</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1900,7 +1900,7 @@
         <v>111</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1913,7 +1913,7 @@
         <v>111</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1926,7 +1926,7 @@
         <v>111</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1952,7 +1952,7 @@
         <v>111</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1965,7 +1965,7 @@
         <v>111</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,7 +1978,7 @@
         <v>111</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1991,7 +1991,7 @@
         <v>111</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2004,7 +2004,7 @@
         <v>111</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2017,7 +2017,7 @@
         <v>111</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2030,7 +2030,7 @@
         <v>111</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2347,6 +2347,24 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="B53:B62"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="B64:B71"/>
+    <mergeCell ref="A63:A71"/>
     <mergeCell ref="B93:B104"/>
     <mergeCell ref="A92:A104"/>
     <mergeCell ref="B106:B110"/>
@@ -2357,24 +2375,6 @@
     <mergeCell ref="A79:A86"/>
     <mergeCell ref="B88:B91"/>
     <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="B53:B62"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="B64:B71"/>
-    <mergeCell ref="A63:A71"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B9:B18"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
@@ -2397,11 +2397,11 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E18 E20:E30 E32:E43 E45:E62 E64:E78 E80:E91 E93:E104 E106:E1048576" xr:uid="{855525DE-213F-45D8-9587-64AA93ECBAA2}">
       <formula1>"Done,Failed,Not Started,Implemented"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D1048576 D3" xr:uid="{7626D55B-BD6E-40C3-B896-B398F13D069A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{7626D55B-BD6E-40C3-B896-B398F13D069A}">
       <formula1>"Done,Not Started,Failed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Implemented All Test Methods in Data Access Layer
</commit_message>
<xml_diff>
--- a/Progress/DataAccessLayer.xlsx
+++ b/Progress/DataAccessLayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Driving-License-Management-Desktop-App\Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D539E3-10BB-444D-B4A6-4F1810C9A4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58961C2C-903B-4562-8F3B-84A9BECA2C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="118">
   <si>
     <t>Class Name</t>
   </si>
@@ -383,9 +383,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>public static bool GetApplicationInfoByID(int ApplicationID, ref int ApplicantPersonID, ref DateTime ApplicationDate, ref int ApplicationTypeID, ref byte ApplicationStatus,ref DateTime LastStatusDate, ref float PaidFees, ref int CreatedByUserID)</t>
   </si>
   <si>
@@ -395,10 +392,10 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>public static bool DoesPersonHaveUser(int PersonID)</t>
-  </si>
-  <si>
     <t>Implemented</t>
+  </si>
+  <si>
+    <t>public static bool DoesPersonHaveUser44(int PersonID)</t>
   </si>
 </sst>
 </file>
@@ -878,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C107" zoomScale="131" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,7 +905,7 @@
         <v>110</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>112</v>
@@ -940,7 +937,7 @@
         <v>111</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>112</v>
@@ -997,7 +994,7 @@
       <c r="A7" s="13"/>
       <c r="B7" s="10"/>
       <c r="C7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>111</v>
@@ -1023,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>111</v>
@@ -1497,7 +1494,7 @@
         <v>111</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1510,7 +1507,7 @@
         <v>111</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1523,7 +1520,7 @@
         <v>111</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1536,7 +1533,7 @@
         <v>111</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1549,7 +1546,7 @@
         <v>111</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1562,7 +1559,7 @@
         <v>111</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1575,7 +1572,7 @@
         <v>111</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1601,7 +1598,7 @@
         <v>111</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1614,7 +1611,7 @@
         <v>111</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,7 +1624,7 @@
         <v>111</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1640,7 +1637,7 @@
         <v>111</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1653,7 +1650,7 @@
         <v>111</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1666,7 +1663,7 @@
         <v>111</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1679,7 +1676,7 @@
         <v>111</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1692,7 +1689,7 @@
         <v>111</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1705,7 +1702,7 @@
         <v>111</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1718,7 +1715,7 @@
         <v>111</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1744,7 +1741,7 @@
         <v>111</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1757,7 +1754,7 @@
         <v>111</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1770,7 +1767,7 @@
         <v>111</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -1783,7 +1780,7 @@
         <v>111</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1796,7 +1793,7 @@
         <v>111</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1809,7 +1806,7 @@
         <v>111</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1822,7 +1819,7 @@
         <v>111</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1835,7 +1832,7 @@
         <v>111</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1861,7 +1858,7 @@
         <v>111</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1874,7 +1871,7 @@
         <v>111</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1887,7 +1884,7 @@
         <v>111</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1900,7 +1897,7 @@
         <v>111</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1913,7 +1910,7 @@
         <v>111</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1926,7 +1923,7 @@
         <v>111</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1952,7 +1949,7 @@
         <v>111</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1965,7 +1962,7 @@
         <v>111</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,7 +1975,7 @@
         <v>111</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1991,7 +1988,7 @@
         <v>111</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2004,7 +2001,7 @@
         <v>111</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2017,7 +2014,7 @@
         <v>111</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2030,7 +2027,7 @@
         <v>111</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2056,7 +2053,7 @@
         <v>111</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2069,7 +2066,7 @@
         <v>111</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2082,7 +2079,7 @@
         <v>111</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2095,7 +2092,7 @@
         <v>111</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2121,7 +2118,7 @@
         <v>111</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2134,7 +2131,7 @@
         <v>111</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2147,7 +2144,7 @@
         <v>111</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2160,7 +2157,7 @@
         <v>111</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2173,7 +2170,7 @@
         <v>111</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2186,7 +2183,7 @@
         <v>111</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2199,7 +2196,7 @@
         <v>111</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2212,7 +2209,7 @@
         <v>111</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -2225,7 +2222,7 @@
         <v>111</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -2238,7 +2235,7 @@
         <v>111</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -2251,7 +2248,7 @@
         <v>111</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -2264,7 +2261,7 @@
         <v>111</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2290,7 +2287,7 @@
         <v>111</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2303,7 +2300,7 @@
         <v>111</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2316,7 +2313,7 @@
         <v>111</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2329,7 +2326,7 @@
         <v>111</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2342,29 +2339,11 @@
         <v>111</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B9:B18"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="B53:B62"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="B64:B71"/>
-    <mergeCell ref="A63:A71"/>
     <mergeCell ref="B93:B104"/>
     <mergeCell ref="A92:A104"/>
     <mergeCell ref="B106:B110"/>
@@ -2375,6 +2354,24 @@
     <mergeCell ref="A79:A86"/>
     <mergeCell ref="B88:B91"/>
     <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="B53:B62"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="B64:B71"/>
+    <mergeCell ref="A63:A71"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
@@ -2397,7 +2394,7 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E18 E20:E30 E32:E43 E45:E62 E64:E78 E80:E91 E93:E104 E106:E1048576" xr:uid="{855525DE-213F-45D8-9587-64AA93ECBAA2}">
       <formula1>"Done,Failed,Not Started,Implemented"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Testing Data Access Layer Done
</commit_message>
<xml_diff>
--- a/Progress/DataAccessLayer.xlsx
+++ b/Progress/DataAccessLayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Driving-License-Management-Desktop-App\Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A2F011-6A82-41BF-8848-A02E965F3845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201CF333-7E39-453C-AD0A-389746937397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1152" windowWidth="16608" windowHeight="8616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="117">
   <si>
     <t>Class Name</t>
   </si>
@@ -392,13 +392,7 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>Implemented</t>
-  </si>
-  <si>
     <t>public static bool DoesPersonHaveUser44(int PersonID)</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -878,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="81" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,7 +958,7 @@
       </c>
       <c r="J4" s="9">
         <f>(COUNTIF(E2:E999,"Done"))/(COUNTIF(E2:E999,"Done") + COUNTIF(E2:E999,"Not Started") + COUNTIF(E2:E999,"Implemented") + COUNTIF(E2:E999,"Failed"))</f>
-        <v>0.66315789473684206</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1874,7 +1868,7 @@
         <v>111</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1900,7 +1894,7 @@
         <v>111</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1913,7 +1907,7 @@
         <v>111</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1926,7 +1920,7 @@
         <v>111</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1952,7 +1946,7 @@
         <v>111</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1965,7 +1959,7 @@
         <v>111</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,7 +1972,7 @@
         <v>111</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1991,7 +1985,7 @@
         <v>111</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2004,7 +1998,7 @@
         <v>111</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2017,7 +2011,7 @@
         <v>111</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2030,7 +2024,7 @@
         <v>111</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2056,7 +2050,7 @@
         <v>111</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2069,7 +2063,7 @@
         <v>111</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2082,7 +2076,7 @@
         <v>111</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2095,7 +2089,7 @@
         <v>111</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2121,7 +2115,7 @@
         <v>111</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2134,7 +2128,7 @@
         <v>111</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2147,7 +2141,7 @@
         <v>111</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2160,7 +2154,7 @@
         <v>111</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2173,7 +2167,7 @@
         <v>111</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2186,7 +2180,7 @@
         <v>111</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2199,7 +2193,7 @@
         <v>111</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2212,7 +2206,7 @@
         <v>111</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -2225,7 +2219,7 @@
         <v>111</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -2238,20 +2232,20 @@
         <v>111</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
       <c r="B103" s="10"/>
       <c r="C103" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>111</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -2264,7 +2258,7 @@
         <v>111</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2290,7 +2284,7 @@
         <v>111</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2303,7 +2297,7 @@
         <v>111</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2316,7 +2310,7 @@
         <v>111</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2329,7 +2323,7 @@
         <v>111</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -2342,11 +2336,29 @@
         <v>111</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="B53:B62"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="B64:B71"/>
+    <mergeCell ref="A63:A71"/>
     <mergeCell ref="B93:B104"/>
     <mergeCell ref="A92:A104"/>
     <mergeCell ref="B106:B110"/>
@@ -2357,24 +2369,6 @@
     <mergeCell ref="A79:A86"/>
     <mergeCell ref="B88:B91"/>
     <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="B53:B62"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="B64:B71"/>
-    <mergeCell ref="A63:A71"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B9:B18"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">

</xml_diff>